<commit_message>
more changes for exp 3
</commit_message>
<xml_diff>
--- a/3rd_experiment/avl_insert_time_vs_inversions_2025-05-29.xlsx
+++ b/3rd_experiment/avl_insert_time_vs_inversions_2025-05-29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,74 +447,74 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.40964</v>
+        <v>0.081928</v>
       </c>
       <c r="B2" t="n">
-        <v>0.05659423800170771</v>
+        <v>0.02525817399873631</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.491568</v>
+        <v>0.163856</v>
       </c>
       <c r="B3" t="n">
-        <v>0.05701587200019276</v>
+        <v>0.02543574199808063</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.655424</v>
+        <v>0.245784</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05767472499792348</v>
+        <v>0.02524120299494825</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.737352</v>
+        <v>0.901209</v>
       </c>
       <c r="B5" t="n">
-        <v>0.05710090299908188</v>
+        <v>0.02510983100364683</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.901209</v>
+        <v>0.983137</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05635653399804141</v>
+        <v>0.02586906700162217</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.983137</v>
+        <v>1.065065</v>
       </c>
       <c r="B7" t="n">
-        <v>0.05777700600083335</v>
+        <v>0.02542278699547751</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.065065</v>
+        <v>1.310849</v>
       </c>
       <c r="B8" t="n">
-        <v>0.05747401799817453</v>
+        <v>0.02564401899871882</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.310849</v>
+        <v>1.392777</v>
       </c>
       <c r="B9" t="n">
-        <v>0.05841607700131135</v>
+        <v>0.02543641599913826</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.638561</v>
+        <v>1.884346</v>
       </c>
       <c r="B10" t="n">
-        <v>0.05727761499656481</v>
+        <v>0.02434378200268839</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>2.13013</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0572428769992257</v>
+        <v>0.0250395330003812</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>2.212058</v>
       </c>
       <c r="B12" t="n">
-        <v>0.05757517299934989</v>
+        <v>0.02640118500130484</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>2.375914</v>
       </c>
       <c r="B13" t="n">
-        <v>0.05719281900019269</v>
+        <v>0.02666043900535442</v>
       </c>
     </row>
     <row r="14">
@@ -546,39 +546,39 @@
         <v>2.457842</v>
       </c>
       <c r="B14" t="n">
-        <v>0.05789491299947258</v>
+        <v>0.02645270300126867</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.031339</v>
+        <v>2.621698</v>
       </c>
       <c r="B15" t="n">
-        <v>0.056753741002467</v>
+        <v>0.02654777800489683</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.277123</v>
+        <v>2.703627</v>
       </c>
       <c r="B16" t="n">
-        <v>0.05770721400040202</v>
+        <v>0.02665507500205422</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.359051</v>
+        <v>3.031339</v>
       </c>
       <c r="B17" t="n">
-        <v>0.05722579099892755</v>
+        <v>0.02583294400392333</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3.522908</v>
+        <v>3.359051</v>
       </c>
       <c r="B18" t="n">
-        <v>0.05674196499967366</v>
+        <v>0.02537747300084447</v>
       </c>
     </row>
     <row r="19">
@@ -586,415 +586,415 @@
         <v>3.604836</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0558287410021876</v>
+        <v>0.0258221969997976</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3.686764</v>
+        <v>3.768692</v>
       </c>
       <c r="B20" t="n">
-        <v>0.06263163900075597</v>
+        <v>0.02522520600177813</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.768692</v>
+        <v>3.85062</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0578225460012618</v>
+        <v>0.02532092900219141</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3.85062</v>
+        <v>4.014476</v>
       </c>
       <c r="B22" t="n">
-        <v>0.05758810300176265</v>
+        <v>0.02668907799670706</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>4.178332</v>
+        <v>4.506045</v>
       </c>
       <c r="B23" t="n">
-        <v>0.05674060399906011</v>
+        <v>0.02538750600069761</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>4.424117</v>
+        <v>4.669901</v>
       </c>
       <c r="B24" t="n">
-        <v>0.05640251799923135</v>
+        <v>0.02610378600365948</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4.506045</v>
+        <v>4.751829</v>
       </c>
       <c r="B25" t="n">
-        <v>0.05745102799846791</v>
+        <v>0.02618399700440932</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4.669901</v>
+        <v>4.997613</v>
       </c>
       <c r="B26" t="n">
-        <v>0.05747330400117789</v>
+        <v>0.02570776799984742</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>4.751829</v>
+        <v>5.243397</v>
       </c>
       <c r="B27" t="n">
-        <v>0.05711944199720165</v>
+        <v>0.02638006699999096</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>5.161469</v>
+        <v>5.325326</v>
       </c>
       <c r="B28" t="n">
-        <v>0.05708460299865692</v>
+        <v>0.02556784199987305</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>5.489182</v>
+        <v>5.57111</v>
       </c>
       <c r="B29" t="n">
-        <v>0.05667769999854499</v>
+        <v>0.02583414399850881</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>5.57111</v>
+        <v>5.816894</v>
       </c>
       <c r="B30" t="n">
-        <v>0.05726928700096323</v>
+        <v>0.02595475999987684</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5.734966</v>
+        <v>5.898822</v>
       </c>
       <c r="B31" t="n">
-        <v>0.05745458000092185</v>
+        <v>0.02630334900459275</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>5.816894</v>
+        <v>6.062678</v>
       </c>
       <c r="B32" t="n">
-        <v>0.05699742599972524</v>
+        <v>0.0262667130009504</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>6.718103</v>
+        <v>6.144607</v>
       </c>
       <c r="B33" t="n">
-        <v>0.05757896299837739</v>
+        <v>0.0259565059968736</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7.127744</v>
+        <v>6.390391</v>
       </c>
       <c r="B34" t="n">
-        <v>0.05798635499741067</v>
+        <v>0.02645851299894275</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>7.209672</v>
+        <v>6.472319</v>
       </c>
       <c r="B35" t="n">
-        <v>0.05746753900166368</v>
+        <v>0.02667079800448846</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>7.455456</v>
+        <v>6.718103</v>
       </c>
       <c r="B36" t="n">
-        <v>0.05749376899984782</v>
+        <v>0.02650103299674811</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>7.537384</v>
+        <v>6.963887</v>
       </c>
       <c r="B37" t="n">
-        <v>0.05801967399747809</v>
+        <v>0.02694696399703389</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>7.783168</v>
+        <v>7.127744</v>
       </c>
       <c r="B38" t="n">
-        <v>0.05768146400077967</v>
+        <v>0.02769829500175547</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>8.028953</v>
+        <v>7.209672</v>
       </c>
       <c r="B39" t="n">
-        <v>0.05798772100024507</v>
+        <v>0.0267537270046887</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>8.274737</v>
+        <v>7.2916</v>
       </c>
       <c r="B40" t="n">
-        <v>0.05789852999805589</v>
+        <v>0.02733118700416526</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>8.438592999999999</v>
+        <v>7.537384</v>
       </c>
       <c r="B41" t="n">
-        <v>0.05834912200225517</v>
+        <v>0.02851465599815128</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>8.602449</v>
+        <v>7.619312</v>
       </c>
       <c r="B42" t="n">
-        <v>0.05887824299861677</v>
+        <v>0.02950993299600668</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>8.684377</v>
+        <v>7.783168</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0576098040000943</v>
+        <v>0.03180854800302768</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>8.930161999999999</v>
+        <v>7.865096</v>
       </c>
       <c r="B44" t="n">
-        <v>0.05883203899793443</v>
+        <v>0.03074928199930582</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>9.012090000000001</v>
+        <v>8.028953</v>
       </c>
       <c r="B45" t="n">
-        <v>0.05974932599929161</v>
+        <v>0.03147868000087328</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>9.175946</v>
+        <v>8.356665</v>
       </c>
       <c r="B46" t="n">
-        <v>0.05948081300084596</v>
+        <v>0.03118221999466186</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>9.257873999999999</v>
+        <v>8.438592999999999</v>
       </c>
       <c r="B47" t="n">
-        <v>0.05950909400053206</v>
+        <v>0.02955734500574181</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>9.42173</v>
+        <v>8.602449</v>
       </c>
       <c r="B48" t="n">
-        <v>0.06051565900270361</v>
+        <v>0.03141222600243054</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>9.503658</v>
+        <v>8.684377</v>
       </c>
       <c r="B49" t="n">
-        <v>0.06009252600051695</v>
+        <v>0.0302616230037529</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>9.749442999999999</v>
+        <v>9.503658</v>
       </c>
       <c r="B50" t="n">
-        <v>0.05894160599928</v>
+        <v>0.03110415799892507</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>9.831371000000001</v>
+        <v>9.995227</v>
       </c>
       <c r="B51" t="n">
-        <v>0.06003833900103928</v>
+        <v>0.03078853199986042</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>10.73258</v>
+        <v>10.241011</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0584186240012059</v>
+        <v>0.0316529060000903</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>11.14222</v>
+        <v>10.322939</v>
       </c>
       <c r="B53" t="n">
-        <v>0.05886736799948267</v>
+        <v>0.03194444199471036</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>11.388005</v>
+        <v>10.650652</v>
       </c>
       <c r="B54" t="n">
-        <v>0.05940402600026573</v>
+        <v>0.03093208099744515</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>11.551861</v>
+        <v>10.73258</v>
       </c>
       <c r="B55" t="n">
-        <v>0.05901128700133995</v>
+        <v>0.02972358599799918</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>11.715717</v>
+        <v>10.896436</v>
       </c>
       <c r="B56" t="n">
-        <v>0.05868324999755714</v>
+        <v>0.03225036799994996</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>11.961501</v>
+        <v>12.043429</v>
       </c>
       <c r="B57" t="n">
-        <v>0.05990851200112957</v>
+        <v>0.02924031800648663</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>12.043429</v>
+        <v>12.534998</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0590109439981461</v>
+        <v>0.03001804900122806</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>12.125357</v>
+        <v>12.616926</v>
       </c>
       <c r="B59" t="n">
-        <v>0.05954758300140384</v>
+        <v>0.03015428299841005</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>12.534998</v>
+        <v>12.86271</v>
       </c>
       <c r="B60" t="n">
-        <v>0.06067451600029017</v>
+        <v>0.0281556210029521</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>12.86271</v>
+        <v>13.272351</v>
       </c>
       <c r="B61" t="n">
-        <v>0.05942923299880931</v>
+        <v>0.02966268199816113</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>12.944638</v>
+        <v>13.436207</v>
       </c>
       <c r="B62" t="n">
-        <v>0.06133386600049562</v>
+        <v>0.02974016799998935</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>13.436207</v>
+        <v>13.518135</v>
       </c>
       <c r="B63" t="n">
-        <v>0.06109478299913462</v>
+        <v>0.03018881700700149</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>13.518135</v>
+        <v>14.009704</v>
       </c>
       <c r="B64" t="n">
-        <v>0.06239366400041035</v>
+        <v>0.0299486580042867</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>13.681991</v>
+        <v>14.091632</v>
       </c>
       <c r="B65" t="n">
-        <v>0.06328204100282164</v>
+        <v>0.03040733800298767</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>13.763919</v>
+        <v>14.255488</v>
       </c>
       <c r="B66" t="n">
-        <v>0.06359657799839624</v>
+        <v>0.03009416799613973</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>13.845847</v>
+        <v>14.337416</v>
       </c>
       <c r="B67" t="n">
-        <v>0.06867352799963555</v>
+        <v>0.03006054500292521</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>15.238625</v>
+        <v>14.419344</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0620187079985044</v>
+        <v>0.03085615799500374</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>15.484409</v>
+        <v>14.910913</v>
       </c>
       <c r="B69" t="n">
-        <v>0.06161129299653112</v>
+        <v>0.03079165399685735</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>15.648265</v>
+        <v>15.238625</v>
       </c>
       <c r="B70" t="n">
-        <v>0.06163882299733814</v>
+        <v>0.03033495199633762</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>15.730193</v>
       </c>
       <c r="B71" t="n">
-        <v>0.06342450699958135</v>
+        <v>0.03079555999283912</v>
       </c>
     </row>
     <row r="72">
@@ -1010,271 +1010,295 @@
         <v>15.812122</v>
       </c>
       <c r="B72" t="n">
-        <v>0.06292001899782917</v>
+        <v>0.02989649200026179</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>16.385618</v>
+        <v>16.30369</v>
       </c>
       <c r="B73" t="n">
-        <v>0.06159728700004052</v>
+        <v>0.03123082999809412</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>16.877187</v>
+        <v>16.385618</v>
       </c>
       <c r="B74" t="n">
-        <v>0.06216970500099706</v>
+        <v>0.03011389399762265</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>16.959115</v>
+        <v>16.631403</v>
       </c>
       <c r="B75" t="n">
-        <v>0.06305909100046847</v>
+        <v>0.03096671800449258</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>17.122971</v>
+        <v>16.959115</v>
       </c>
       <c r="B76" t="n">
-        <v>0.06367795200276305</v>
+        <v>0.03074913100135745</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>17.204899</v>
+        <v>17.122971</v>
       </c>
       <c r="B77" t="n">
-        <v>0.06240590399829671</v>
+        <v>0.03169431500282371</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>17.368755</v>
+        <v>17.204899</v>
       </c>
       <c r="B78" t="n">
-        <v>0.06161676099873148</v>
+        <v>0.03118541800358798</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>17.696468</v>
+        <v>17.368755</v>
       </c>
       <c r="B79" t="n">
-        <v>0.06515662200035877</v>
+        <v>0.03179089300101623</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>18.02418</v>
+        <v>17.450683</v>
       </c>
       <c r="B80" t="n">
-        <v>0.06515223400128889</v>
+        <v>0.03304675900290022</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>18.188036</v>
+        <v>17.778396</v>
       </c>
       <c r="B81" t="n">
-        <v>0.06374985999718774</v>
+        <v>0.03275902600580594</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>18.515749</v>
+        <v>18.02418</v>
       </c>
       <c r="B82" t="n">
-        <v>0.06596412299768417</v>
+        <v>0.03175470499991206</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>18.597677</v>
+        <v>18.188036</v>
       </c>
       <c r="B83" t="n">
-        <v>0.06435208299808437</v>
+        <v>0.0319614459949662</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>18.761533</v>
+        <v>18.515749</v>
       </c>
       <c r="B84" t="n">
-        <v>0.06511443600174971</v>
+        <v>0.03142127099999925</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>18.843461</v>
+        <v>18.597677</v>
       </c>
       <c r="B85" t="n">
-        <v>0.06730166299894336</v>
+        <v>0.03270616899681045</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>18.925389</v>
+        <v>18.761533</v>
       </c>
       <c r="B86" t="n">
-        <v>0.06811041599939927</v>
+        <v>0.03273856099986006</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>19.089245</v>
+        <v>18.843461</v>
       </c>
       <c r="B87" t="n">
-        <v>0.06857625299744541</v>
+        <v>0.03356986599828815</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>19.171173</v>
+        <v>18.925389</v>
       </c>
       <c r="B88" t="n">
-        <v>0.0648568479991809</v>
+        <v>0.03294246699806536</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>19.662742</v>
+        <v>19.416958</v>
       </c>
       <c r="B89" t="n">
-        <v>0.06855258799987496</v>
+        <v>0.03448192699579522</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>19.74467</v>
+        <v>19.498886</v>
       </c>
       <c r="B90" t="n">
-        <v>0.06722179100324865</v>
+        <v>0.03377556299528806</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>19.990454</v>
+        <v>19.662742</v>
       </c>
       <c r="B91" t="n">
-        <v>0.07108045399945695</v>
+        <v>0.03487447099905694</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>20.072382</v>
+        <v>19.74467</v>
       </c>
       <c r="B92" t="n">
-        <v>0.06954706400210853</v>
+        <v>0.03408476799813798</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>20.236239</v>
+        <v>19.990454</v>
       </c>
       <c r="B93" t="n">
-        <v>0.07026728300115792</v>
+        <v>0.03873087400279474</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>20.318167</v>
+        <v>20.072382</v>
       </c>
       <c r="B94" t="n">
-        <v>0.07005782499982161</v>
+        <v>0.03704707400174811</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>21.05552</v>
+        <v>20.482023</v>
       </c>
       <c r="B95" t="n">
-        <v>0.07170280500213266</v>
+        <v>0.04039318600553088</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>21.137448</v>
+        <v>20.563951</v>
       </c>
       <c r="B96" t="n">
-        <v>0.07067124300010619</v>
+        <v>0.04061458000069251</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>21.46516</v>
+        <v>20.645879</v>
       </c>
       <c r="B97" t="n">
-        <v>0.0747001139970962</v>
+        <v>0.0382942619980895</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>21.629016</v>
+        <v>20.809735</v>
       </c>
       <c r="B98" t="n">
-        <v>0.07242836099976557</v>
+        <v>0.04105730000446783</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>21.710944</v>
+        <v>20.891663</v>
       </c>
       <c r="B99" t="n">
-        <v>0.07489457299743663</v>
+        <v>0.04221983200113755</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>21.956729</v>
+        <v>21.629016</v>
       </c>
       <c r="B100" t="n">
-        <v>0.07462113500150735</v>
+        <v>0.04121946400118759</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>23.021794</v>
+        <v>21.710944</v>
       </c>
       <c r="B101" t="n">
-        <v>0.07575315000212868</v>
+        <v>0.04135833100008313</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>23.103722</v>
+        <v>21.874801</v>
       </c>
       <c r="B102" t="n">
-        <v>0.07729083999947761</v>
+        <v>0.04122477499913657</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>23.18565</v>
+        <v>22.448297</v>
       </c>
       <c r="B103" t="n">
-        <v>0.08013372200002777</v>
+        <v>0.0412707750001573</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>23.923003</v>
+        <v>22.530225</v>
       </c>
       <c r="B104" t="n">
-        <v>0.08301723399927141</v>
+        <v>0.04085884999949485</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>24.004931</v>
+        <v>22.612153</v>
       </c>
       <c r="B105" t="n">
-        <v>0.08158079399800044</v>
+        <v>0.04125330100214342</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>23.103722</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.0421513299952494</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>23.18565</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0.04345248600293417</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>23.677219</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0.04343833099846961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>